<commit_message>
tidied up excel files but do not understand reps
</commit_message>
<xml_diff>
--- a/Sample of Density Protocol.xlsx
+++ b/Sample of Density Protocol.xlsx
@@ -1,34 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariozuliani/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="53">
   <si>
     <t>Shrub ID</t>
   </si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>SS9</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Mojave</t>
   </si>
 </sst>
 </file>
@@ -229,17 +229,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -295,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -330,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -507,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,18 +523,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,25 +548,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -569,28 +580,31 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>34.697800000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-115.68685000000001</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.3</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.7</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -601,28 +615,31 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>34.697809999999997</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-115.68387</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="I3">
-        <v>0.9</v>
       </c>
       <c r="J3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -633,28 +650,31 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>34.697809999999997</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>-115.68387</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.7</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.6</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -665,28 +685,31 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>34.697809999999997</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>-115.68388</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.6</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -697,28 +720,31 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>34.69782</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>-115.68388</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.55000000000000004</v>
-      </c>
-      <c r="I6">
-        <v>0.3</v>
       </c>
       <c r="J6">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -729,28 +755,31 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>34.697809999999997</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-115.68391</v>
-      </c>
-      <c r="H7">
-        <v>0.6</v>
       </c>
       <c r="I7">
         <v>0.6</v>
       </c>
       <c r="J7">
+        <v>0.6</v>
+      </c>
+      <c r="K7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -761,28 +790,31 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>34.697279999999999</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>-115.68394000000001</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>2.1</v>
-      </c>
-      <c r="I8">
-        <v>1.9</v>
       </c>
       <c r="J8">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -793,28 +825,31 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>34.697769999999998</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>-115.68392</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.8</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -825,28 +860,31 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>34.697760000000002</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-115.68394000000001</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.5</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.4</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -857,28 +895,31 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
         <v>25</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>34.697760000000002</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>-115.68392</v>
-      </c>
-      <c r="H11">
-        <v>0.4</v>
       </c>
       <c r="I11">
         <v>0.4</v>
       </c>
       <c r="J11">
+        <v>0.4</v>
+      </c>
+      <c r="K11">
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -889,28 +930,31 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>34.697740000000003</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>-115.68394000000001</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.9</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.8</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -921,28 +965,31 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
         <v>25</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>34.697719999999997</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>-115.68395</v>
-      </c>
-      <c r="H13">
-        <v>0.6</v>
       </c>
       <c r="I13">
         <v>0.6</v>
       </c>
       <c r="J13">
+        <v>0.6</v>
+      </c>
+      <c r="K13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -953,28 +1000,31 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
         <v>25</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>34.69773</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>-115.68392</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.5</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.4</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -985,28 +1035,31 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>34.697719999999997</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>-115.68394000000001</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.4</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.3</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1017,28 +1070,31 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>34.697719999999997</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>-115.68393</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>1</v>
-      </c>
-      <c r="I16">
-        <v>0.7</v>
       </c>
       <c r="J16">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1049,28 +1105,31 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
         <v>26</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>34.697710000000001</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>-115.68391</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.6</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.4</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1081,28 +1140,31 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
         <v>25</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>34.697719999999997</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>-115.68391</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.3</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>0.25</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1113,28 +1175,31 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>34.697719999999997</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>-115.68391</v>
-      </c>
-      <c r="H19">
-        <v>0.5</v>
       </c>
       <c r="I19">
         <v>0.5</v>
       </c>
       <c r="J19">
+        <v>0.5</v>
+      </c>
+      <c r="K19">
         <v>0.45</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1145,28 +1210,31 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
         <v>25</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>34.69773</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>-115.68388</v>
-      </c>
-      <c r="H20">
-        <v>0.3</v>
       </c>
       <c r="I20">
         <v>0.3</v>
       </c>
       <c r="J20">
+        <v>0.3</v>
+      </c>
+      <c r="K20">
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1177,28 +1245,31 @@
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
         <v>25</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>34.69773</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>-115.68388</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>0.6</v>
-      </c>
-      <c r="I21">
-        <v>0.5</v>
       </c>
       <c r="J21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1209,28 +1280,31 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>34.697749999999999</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>-115.68388</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>1.3</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>1.2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1241,28 +1315,31 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
         <v>25</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>34.697769999999998</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>-115.68387</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>0.5</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>0.45</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1273,19 +1350,19 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
         <v>25</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>34.697749999999999</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>-115.68383</v>
-      </c>
-      <c r="H24">
-        <v>0.4</v>
       </c>
       <c r="I24">
         <v>0.4</v>
@@ -1293,8 +1370,11 @@
       <c r="J24">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1305,28 +1385,31 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
         <v>25</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>34.697740000000003</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>-115.68382</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.5</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>0.4</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1337,28 +1420,31 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
         <v>8</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>34.69773</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>-115.68382</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>1</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>0.95</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1369,28 +1455,31 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
         <v>45</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>8</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>34.206220000000002</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>-115.71937</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>1.3</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>0.8</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>0.65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1401,28 +1490,31 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s">
         <v>45</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>34.206270000000004</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>-115.71941</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>2.1</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>1.73</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>1.6</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1433,28 +1525,31 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" t="s">
         <v>45</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>8</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>34.206299999999999</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>-115.71935000000001</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>1.4</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>1.2</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1465,28 +1560,31 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
         <v>45</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>8</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>34.20626</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>-115.71925</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>2.04</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>1.55</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1497,28 +1595,31 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
         <v>45</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>8</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>34.206209999999999</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>-115.71926999999999</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>0.4</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>0.3</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1529,28 +1630,31 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" t="s">
         <v>45</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>8</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>34.206150000000001</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>-115.71935000000001</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>0.9</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>0.95</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1561,28 +1665,31 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
         <v>45</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>26</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>34.206180000000003</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>-115.71935000000001</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>2.6</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>1.9</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>1.8</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -1593,28 +1700,31 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
         <v>45</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>26</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>34.206105999999998</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>-115.71942</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>1.5</v>
-      </c>
-      <c r="I34">
-        <v>1.3</v>
       </c>
       <c r="J34">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1625,40 +1735,37 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
         <v>45</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>26</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>34.206189999999999</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>-115.71941</v>
-      </c>
-      <c r="H35">
-        <v>2.2000000000000002</v>
       </c>
       <c r="I35">
         <v>2.2000000000000002</v>
       </c>
       <c r="J35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K35">
         <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>